<commit_message>
Contract Summary by POB
</commit_message>
<xml_diff>
--- a/src/java/resources/excel_input_templates/Outputs_Summary_v2.xlsx
+++ b/src/java/resources/excel_input_templates/Outputs_Summary_v2.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>Contract Summary by Pob</t>
   </si>
@@ -104,6 +104,33 @@
   </si>
   <si>
     <t>Contract Summary</t>
+  </si>
+  <si>
+    <t>Percentage-of-Completion POb's</t>
+  </si>
+  <si>
+    <t>Point-in-Time POb's</t>
+  </si>
+  <si>
+    <t>Straight-Line POb's</t>
+  </si>
+  <si>
+    <t>Third Party Commissions</t>
+  </si>
+  <si>
+    <t>Billings To Date</t>
+  </si>
+  <si>
+    <t>Contract Summary Totals</t>
+  </si>
+  <si>
+    <t>Percentage-of-Completion POb Totals</t>
+  </si>
+  <si>
+    <t>Point-in-Time POb Totals</t>
+  </si>
+  <si>
+    <t>Straight-Line POb Totals</t>
   </si>
 </sst>
 </file>
@@ -114,7 +141,7 @@
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="13">
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
@@ -166,8 +193,26 @@
       <sz val="11.0"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="12.0"/>
+      <color rgb="FF000000"/>
+      <name val="Trebuchet MS"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12.0"/>
+      <color rgb="FF000000"/>
+      <name val="Trebuchet MS"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12.0"/>
+      <color rgb="FF000000"/>
+      <name val="Trebuchet MS"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -192,8 +237,14 @@
         <bgColor rgb="FFDEEAF6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border/>
     <border>
       <left style="thin">
@@ -301,11 +352,25 @@
         <color rgb="FF000000"/>
       </bottom>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="27">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -354,6 +419,24 @@
     </xf>
     <xf borderId="10" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="11" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="11" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="11" fillId="5" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="11" fillId="5" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="11" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="11" fillId="5" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -543,21 +626,165 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" ht="15.75" customHeight="1"/>
-    <row r="12" ht="15.75" customHeight="1"/>
-    <row r="13" ht="15.75" customHeight="1"/>
-    <row r="14" ht="15.75" customHeight="1"/>
-    <row r="15" ht="15.75" customHeight="1"/>
-    <row r="16" ht="15.75" customHeight="1"/>
-    <row r="17" ht="15.75" customHeight="1"/>
-    <row r="18" ht="15.75" customHeight="1"/>
-    <row r="19" ht="15.75" customHeight="1"/>
-    <row r="20" ht="15.75" customHeight="1"/>
-    <row r="21" ht="15.75" customHeight="1"/>
-    <row r="22" ht="15.75" customHeight="1"/>
-    <row r="23" ht="15.75" customHeight="1"/>
-    <row r="24" ht="15.75" customHeight="1"/>
-    <row r="25" ht="15.75" customHeight="1"/>
+    <row r="11" ht="15.75" customHeight="1">
+      <c r="A11" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+    </row>
+    <row r="12" ht="15.75" customHeight="1">
+      <c r="A12" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+    </row>
+    <row r="13" ht="15.75" customHeight="1">
+      <c r="A13" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+    </row>
+    <row r="14" ht="15.75" customHeight="1">
+      <c r="A14" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+    </row>
+    <row r="15" ht="15.75" customHeight="1">
+      <c r="A15" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+    </row>
+    <row r="16" ht="15.75" customHeight="1">
+      <c r="A16" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+    </row>
+    <row r="17" ht="15.75" customHeight="1">
+      <c r="A17" s="25"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+    </row>
+    <row r="18" ht="15.75" customHeight="1">
+      <c r="A18" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+    </row>
+    <row r="19" ht="15.75" customHeight="1">
+      <c r="A19" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+    </row>
+    <row r="20" ht="15.75" customHeight="1">
+      <c r="A20" s="25"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+    </row>
+    <row r="21" ht="15.75" customHeight="1">
+      <c r="A21" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+    </row>
+    <row r="22" ht="15.75" customHeight="1">
+      <c r="A22" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+    </row>
+    <row r="23" ht="15.75" customHeight="1">
+      <c r="A23" s="25"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+    </row>
+    <row r="24" ht="15.75" customHeight="1">
+      <c r="A24" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
+    </row>
+    <row r="25" ht="15.75" customHeight="1">
+      <c r="A25" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="22"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
+    </row>
     <row r="26" ht="15.75" customHeight="1"/>
     <row r="27" ht="15.75" customHeight="1"/>
     <row r="28" ht="15.75" customHeight="1"/>
@@ -1516,6 +1743,23 @@
     <row r="981" ht="15.75" customHeight="1"/>
     <row r="982" ht="15.75" customHeight="1"/>
     <row r="983" ht="15.75" customHeight="1"/>
+    <row r="984" ht="15.75" customHeight="1"/>
+    <row r="985" ht="15.75" customHeight="1"/>
+    <row r="986" ht="15.75" customHeight="1"/>
+    <row r="987" ht="15.75" customHeight="1"/>
+    <row r="988" ht="15.75" customHeight="1"/>
+    <row r="989" ht="15.75" customHeight="1"/>
+    <row r="990" ht="15.75" customHeight="1"/>
+    <row r="991" ht="15.75" customHeight="1"/>
+    <row r="992" ht="15.75" customHeight="1"/>
+    <row r="993" ht="15.75" customHeight="1"/>
+    <row r="994" ht="15.75" customHeight="1"/>
+    <row r="995" ht="15.75" customHeight="1"/>
+    <row r="996" ht="15.75" customHeight="1"/>
+    <row r="997" ht="15.75" customHeight="1"/>
+    <row r="998" ht="15.75" customHeight="1"/>
+    <row r="999" ht="15.75" customHeight="1"/>
+    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A7:A8"/>

</xml_diff>